<commit_message>
dokumentasjon brukt under kick-off med KV.
</commit_message>
<xml_diff>
--- a/doc/le_nb_iot_controller_ModuleReviewChecklist.xlsx
+++ b/doc/le_nb_iot_controller_ModuleReviewChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.rune.herheim\Documents\GitHub\NBIOT_RADIO_SYSTEM\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.rune.herheim\Dropbox (Lillebakk)\Lillebakk Team\herheim\Documents\GitHub\LE_NB_IOT_CONTROLLER\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Frode Sundal - Personal View" guid="{BB5EAECB-8EEF-4DE2-9C73-C75A1E03B482}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1596" windowHeight="1028" activeSheetId="3"/>
+    <customWorkbookView name="  - Personal View" guid="{DB10AD2D-E6B8-47D9-A473-F38D6906B0B5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="728" activeSheetId="6"/>
     <customWorkbookView name="Schabel, Stefan - Personal View" guid="{24287BB4-78F5-41D1-8279-0065565E5B4E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1184" tabRatio="826" activeSheetId="1"/>
-    <customWorkbookView name="  - Personal View" guid="{DB10AD2D-E6B8-47D9-A473-F38D6906B0B5}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="728" activeSheetId="6"/>
-    <customWorkbookView name="Frode Sundal - Personal View" guid="{BB5EAECB-8EEF-4DE2-9C73-C75A1E03B482}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1596" windowHeight="1028" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="334">
   <si>
     <t>Comment</t>
   </si>
@@ -1402,13 +1402,88 @@
     <t>Statnett is their customer again.</t>
   </si>
   <si>
-    <t>NOK2000</t>
-  </si>
-  <si>
     <t>for a demo version</t>
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All actions are given in this document: </t>
+  </si>
+  <si>
+    <t>..\..\..\customers\kjeller vindteknikk\actions lastmåler.xlsx</t>
+  </si>
+  <si>
+    <t>NB will not be available before testing of concept 1</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>KV + LE, 02.06.2017</t>
+  </si>
+  <si>
+    <t>NB will not be available before testing of concept 2</t>
+  </si>
+  <si>
+    <t>Short lifetime due battery drain by GPRS module.</t>
+  </si>
+  <si>
+    <t>Need to make a pilot with GPRS support instead of NB.</t>
+  </si>
+  <si>
+    <t>Product development might be terminated due to short lifetime.</t>
+  </si>
+  <si>
+    <t>Make a low power GPRS solution, and push for NB.</t>
+  </si>
+  <si>
+    <t>02.06.2017</t>
+  </si>
+  <si>
+    <t>Kick-off review at Kjeller Vindteknikk.</t>
+  </si>
+  <si>
+    <t>..\..\LE_LPWAN_SYSTEM\doc\lpwan_system_requirement.docx</t>
+  </si>
+  <si>
+    <t>300k + 200k</t>
+  </si>
+  <si>
+    <t>300k for concept 0 (spec), and 200k for concept 1 (pilot)</t>
+  </si>
+  <si>
+    <t>Requirements covered in the specification is accepted. The SRD is currently only reviewed by JRH:</t>
+  </si>
+  <si>
+    <t>Currently a GSM/GPRS (2G) solution is considred, but uses to much current while in sleep. Or too long power down time wrt requested report rate.</t>
+  </si>
+  <si>
+    <t>Jan Rune Herheim</t>
+  </si>
+  <si>
+    <t>Kick-off at Kjeller Vindteknikk.</t>
+  </si>
+  <si>
+    <t>Only by JRH</t>
+  </si>
+  <si>
+    <t>Still open actions, but not wrt SRD.</t>
+  </si>
+  <si>
+    <t>Will be updated later.</t>
+  </si>
+  <si>
+    <t>Bjørn Egil Nygaard</t>
+  </si>
+  <si>
+    <t>Finn Nyhammer</t>
+  </si>
+  <si>
+    <t>Andre Lillebakk</t>
+  </si>
+  <si>
+    <t>Halfdan Agustsson</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2701,27 +2776,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2738,6 +2805,15 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5653,15 +5729,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>4763</xdr:colOff>
           <xdr:row>68</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>3867150</xdr:colOff>
-          <xdr:row>86</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:colOff>3829050</xdr:colOff>
+          <xdr:row>120</xdr:row>
+          <xdr:rowOff>147638</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6373,13 +6449,13 @@
       <c r="C20" s="60" t="s">
         <v>287</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="35" t="str">
         <f>'System R'!C4</f>
-        <v>1</v>
+        <v>02.06.2017</v>
       </c>
       <c r="E20" s="48" t="str">
         <f>'System R'!C5</f>
-        <v>no</v>
+        <v>yes</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
@@ -6387,13 +6463,13 @@
       <c r="C21" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="35" t="str">
         <f>'Specification R'!C4</f>
-        <v>2</v>
+        <v>02.06.2017</v>
       </c>
       <c r="E21" s="48" t="str">
         <f>'Specification R'!C5</f>
-        <v>no</v>
+        <v>yes</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
@@ -6477,7 +6553,7 @@
       </c>
       <c r="D28" s="169" t="str">
         <f>'System R'!C12</f>
-        <v>NOK2000</v>
+        <v>300k + 200k</v>
       </c>
       <c r="E28" s="38">
         <f>'Final Design&amp;Layout R'!C10</f>
@@ -6553,7 +6629,7 @@
       <c r="C35" s="71"/>
       <c r="D35" s="211">
         <f>COUNTIF(Risks!B2:B1000,"*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E35" s="37"/>
     </row>
@@ -6605,7 +6681,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -6663,9 +6739,6 @@
       <c r="I3" s="93"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
       <c r="B4" s="32"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -6676,9 +6749,6 @@
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -6689,9 +6759,6 @@
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>3</v>
-      </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -6738,7 +6805,9 @@
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -6751,7 +6820,9 @@
       <c r="F10" s="12"/>
       <c r="G10" s="32"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="I10" s="235" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -6984,6 +7055,9 @@
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -6998,7 +7072,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7006,7 +7080,7 @@
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="4" width="54.3984375" customWidth="1"/>
     <col min="5" max="5" width="14.86328125" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -7033,24 +7107,40 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>310</v>
+      </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>315</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>313</v>
+      </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>316</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>317</v>
+      </c>
+      <c r="E3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -7098,7 +7188,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9:C10"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7121,9 +7211,9 @@
         <f>OVERVIEW!D7</f>
         <v>NB IoT Radio</v>
       </c>
-      <c r="D1" s="123">
+      <c r="D1" s="123" t="str">
         <f>C4</f>
-        <v>1</v>
+        <v>02.06.2017</v>
       </c>
       <c r="E1" s="107"/>
       <c r="F1" s="107"/>
@@ -7149,8 +7239,11 @@
       <c r="B4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="120">
-        <v>1</v>
+      <c r="C4" s="120" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="181" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -7158,7 +7251,7 @@
         <v>101</v>
       </c>
       <c r="C5" s="221" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D5" s="224"/>
       <c r="E5" s="130"/>
@@ -7193,18 +7286,20 @@
       <c r="B9" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="C9" s="228" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="226"/>
+      <c r="C9" s="226" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" s="236" t="s">
+        <v>320</v>
+      </c>
       <c r="E9" s="130"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="229"/>
-      <c r="D10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="237"/>
       <c r="E10" s="130"/>
     </row>
     <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -7223,9 +7318,11 @@
         <v>272</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>306</v>
-      </c>
-      <c r="D12" s="185"/>
+        <v>321</v>
+      </c>
+      <c r="D12" s="185" t="s">
+        <v>322</v>
+      </c>
       <c r="E12" s="129"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -7236,7 +7333,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="186" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E13" s="128"/>
     </row>
@@ -7245,10 +7342,10 @@
         <v>280</v>
       </c>
       <c r="C14" s="126" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D14" s="185" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E14" s="127"/>
     </row>
@@ -7292,14 +7389,16 @@
       <c r="E18" s="108"/>
       <c r="F18" s="108"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B19" s="97" t="s">
         <v>283</v>
       </c>
       <c r="C19" s="221" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="185"/>
+        <v>311</v>
+      </c>
+      <c r="D19" s="185" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="102" t="s">
@@ -7333,7 +7432,9 @@
       <c r="B24" s="101" t="s">
         <v>286</v>
       </c>
-      <c r="C24" s="219"/>
+      <c r="C24" s="219" t="s">
+        <v>324</v>
+      </c>
       <c r="D24" s="220"/>
     </row>
     <row r="25" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.35">
@@ -7359,7 +7460,7 @@
         <v>109</v>
       </c>
       <c r="C27" s="132" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D27" s="186"/>
       <c r="E27" s="130"/>
@@ -7369,7 +7470,7 @@
         <v>110</v>
       </c>
       <c r="C28" s="132" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D28" s="188"/>
       <c r="E28" s="130"/>
@@ -7403,12 +7504,20 @@
       <c r="E31" s="82"/>
       <c r="F31" s="82"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B32" s="106"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="190"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
+      <c r="C32" s="112" t="s">
+        <v>325</v>
+      </c>
+      <c r="D32" s="190" t="s">
+        <v>311</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>311</v>
+      </c>
+      <c r="F32" s="83" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B33" s="104"/>
@@ -7615,16 +7724,19 @@
       <formula1>"yes, partly, no, n/a"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D9:D10" r:id="rId2" display="..\..\LE_LPWAN_SYSTEM\doc\lpwan_system_requirement.docx"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Word.Document.8" shapeId="8193" r:id="rId5">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
+        <oleObject progId="Word.Document.8" shapeId="8193" r:id="rId6">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -7643,7 +7755,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Word.Document.8" shapeId="8193" r:id="rId5"/>
+        <oleObject progId="Word.Document.8" shapeId="8193" r:id="rId6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -7658,8 +7770,8 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD68"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -7682,9 +7794,9 @@
         <f>OVERVIEW!D7</f>
         <v>NB IoT Radio</v>
       </c>
-      <c r="D1" s="199">
+      <c r="D1" s="199" t="str">
         <f>C4</f>
-        <v>2</v>
+        <v>02.06.2017</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="136" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
@@ -7703,8 +7815,8 @@
       <c r="B4" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="140">
-        <v>2</v>
+      <c r="C4" s="140" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
@@ -7712,18 +7824,20 @@
       <c r="B5" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="230"/>
+      <c r="C5" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" s="229" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A6" s="138"/>
       <c r="B6" s="142" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="231"/>
-      <c r="D6" s="230"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="229"/>
     </row>
     <row r="7" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" s="136" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
@@ -7742,18 +7856,20 @@
       <c r="B9" s="216" t="s">
         <v>288</v>
       </c>
-      <c r="C9" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="230"/>
+      <c r="C9" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" s="229" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="215" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A10" s="145"/>
       <c r="B10" s="147" t="s">
         <v>289</v>
       </c>
-      <c r="C10" s="231"/>
-      <c r="D10" s="230"/>
+      <c r="C10" s="228"/>
+      <c r="D10" s="229"/>
     </row>
     <row r="11" spans="1:4" s="215" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="148"/>
@@ -7765,18 +7881,18 @@
       <c r="B12" s="143" t="s">
         <v>261</v>
       </c>
-      <c r="C12" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="230"/>
+      <c r="C12" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="229"/>
     </row>
     <row r="13" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A13" s="145"/>
       <c r="B13" s="147" t="s">
         <v>262</v>
       </c>
-      <c r="C13" s="231"/>
-      <c r="D13" s="230"/>
+      <c r="C13" s="228"/>
+      <c r="D13" s="229"/>
     </row>
     <row r="14" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="148"/>
@@ -7787,18 +7903,20 @@
       <c r="B15" s="149" t="s">
         <v>290</v>
       </c>
-      <c r="C15" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="230"/>
+      <c r="C15" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" s="229" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="145"/>
       <c r="B16" s="150" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="231"/>
-      <c r="D16" s="230"/>
+      <c r="C16" s="228"/>
+      <c r="D16" s="229"/>
     </row>
     <row r="17" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="148"/>
@@ -7809,25 +7927,25 @@
       <c r="B18" s="148" t="s">
         <v>291</v>
       </c>
-      <c r="C18" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="230"/>
+      <c r="C18" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" s="229"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="147" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="231"/>
-      <c r="D19" s="230"/>
+      <c r="C19" s="228"/>
+      <c r="D19" s="229"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="151"/>
       <c r="B20" s="147" t="s">
         <v>194</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="230"/>
+      <c r="C20" s="228"/>
+      <c r="D20" s="229"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="152"/>
@@ -7851,18 +7969,18 @@
       <c r="B23" s="139" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="230"/>
+      <c r="C23" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D23" s="229"/>
     </row>
     <row r="24" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A24" s="145"/>
       <c r="B24" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="231"/>
-      <c r="D24" s="230"/>
+      <c r="C24" s="228"/>
+      <c r="D24" s="229"/>
     </row>
     <row r="25" spans="1:4" s="215" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="148"/>
@@ -7873,17 +7991,17 @@
       <c r="B26" s="139" t="s">
         <v>168</v>
       </c>
-      <c r="C26" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="230"/>
+      <c r="C26" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D26" s="229"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" s="147" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="231"/>
-      <c r="D27" s="230"/>
+      <c r="C27" s="228"/>
+      <c r="D27" s="229"/>
     </row>
     <row r="28" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="148"/>
@@ -7894,30 +8012,30 @@
       <c r="B29" s="139" t="s">
         <v>195</v>
       </c>
-      <c r="C29" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="230"/>
+      <c r="C29" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D29" s="229"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" s="147" t="s">
         <v>196</v>
       </c>
-      <c r="C30" s="231"/>
-      <c r="D30" s="230"/>
+      <c r="C30" s="228"/>
+      <c r="D30" s="229"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" s="147" t="s">
         <v>197</v>
       </c>
-      <c r="C31" s="231"/>
+      <c r="C31" s="228"/>
       <c r="D31" s="171"/>
     </row>
     <row r="32" spans="1:4" ht="20.65" x14ac:dyDescent="0.35">
       <c r="B32" s="147" t="s">
         <v>198</v>
       </c>
-      <c r="C32" s="231"/>
+      <c r="C32" s="228"/>
       <c r="D32" s="171"/>
     </row>
     <row r="33" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
@@ -7929,17 +8047,17 @@
       <c r="B34" s="139" t="s">
         <v>199</v>
       </c>
-      <c r="C34" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="230"/>
+      <c r="C34" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D34" s="229"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="147" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="231"/>
-      <c r="D35" s="230"/>
+      <c r="C35" s="228"/>
+      <c r="D35" s="229"/>
     </row>
     <row r="36" spans="1:4" s="156" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="155"/>
@@ -7951,17 +8069,19 @@
       <c r="B37" s="139" t="s">
         <v>170</v>
       </c>
-      <c r="C37" s="231" t="s">
+      <c r="C37" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="230"/>
+      <c r="D37" s="229" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="231"/>
-      <c r="D38" s="230"/>
+      <c r="C38" s="228"/>
+      <c r="D38" s="229"/>
     </row>
     <row r="39" spans="1:4" s="156" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="147"/>
@@ -7977,17 +8097,17 @@
       <c r="B41" s="139" t="s">
         <v>201</v>
       </c>
-      <c r="C41" s="231" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="230"/>
+      <c r="C41" s="228" t="s">
+        <v>311</v>
+      </c>
+      <c r="D41" s="229"/>
     </row>
     <row r="42" spans="1:4" s="157" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B42" s="147" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="231"/>
-      <c r="D42" s="230"/>
+      <c r="C42" s="228"/>
+      <c r="D42" s="229"/>
     </row>
     <row r="43" spans="1:4" s="158" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="147"/>
@@ -7998,17 +8118,19 @@
       <c r="B44" s="139" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="231" t="s">
+      <c r="C44" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="230"/>
+      <c r="D44" s="229" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B45" s="147" t="s">
         <v>164</v>
       </c>
-      <c r="C45" s="231"/>
-      <c r="D45" s="230"/>
+      <c r="C45" s="228"/>
+      <c r="D45" s="229"/>
     </row>
     <row r="46" spans="1:4" s="156" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="155"/>
@@ -8032,30 +8154,30 @@
       <c r="B48" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="C48" s="231" t="s">
+      <c r="C48" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="230"/>
+      <c r="D48" s="229"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B49" s="160" t="s">
         <v>203</v>
       </c>
-      <c r="C49" s="231"/>
-      <c r="D49" s="230"/>
+      <c r="C49" s="228"/>
+      <c r="D49" s="229"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B50" s="160" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="231"/>
+      <c r="C50" s="228"/>
       <c r="D50" s="171"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B51" s="160" t="s">
         <v>205</v>
       </c>
-      <c r="C51" s="231"/>
+      <c r="C51" s="228"/>
       <c r="D51" s="171"/>
     </row>
     <row r="52" spans="1:6" s="156" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
@@ -8081,7 +8203,7 @@
         <v>260</v>
       </c>
       <c r="C54" s="217" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D54" s="218"/>
     </row>
@@ -8090,7 +8212,7 @@
         <v>109</v>
       </c>
       <c r="C55" s="154" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D55" s="197"/>
     </row>
@@ -8099,7 +8221,7 @@
         <v>110</v>
       </c>
       <c r="C56" s="154" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D56" s="197"/>
     </row>
@@ -8110,14 +8232,16 @@
       <c r="C57" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="D57" s="197"/>
+      <c r="D57" s="197" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B58" s="143" t="s">
         <v>293</v>
       </c>
       <c r="C58" s="154" t="s">
-        <v>64</v>
+        <v>311</v>
       </c>
       <c r="D58" s="197"/>
     </row>
@@ -8146,38 +8270,82 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B62" s="165"/>
-      <c r="C62" s="163"/>
-      <c r="D62" s="198"/>
-      <c r="E62" s="164"/>
-      <c r="F62" s="164"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C62" s="163" t="s">
+        <v>330</v>
+      </c>
+      <c r="D62" s="198" t="s">
+        <v>311</v>
+      </c>
+      <c r="E62" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="F62" s="164" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B63" s="165"/>
-      <c r="C63" s="163"/>
-      <c r="D63" s="198"/>
-      <c r="E63" s="164"/>
-      <c r="F63" s="164"/>
+      <c r="C63" s="163" t="s">
+        <v>331</v>
+      </c>
+      <c r="D63" s="198" t="s">
+        <v>311</v>
+      </c>
+      <c r="E63" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="F63" s="164" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B64" s="165"/>
-      <c r="C64" s="163"/>
-      <c r="D64" s="198"/>
-      <c r="E64" s="164"/>
-      <c r="F64" s="164"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C64" s="163" t="s">
+        <v>332</v>
+      </c>
+      <c r="D64" s="198" t="s">
+        <v>311</v>
+      </c>
+      <c r="E64" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="F64" s="164" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B65" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="163"/>
-      <c r="D65" s="198"/>
-      <c r="E65" s="164"/>
-      <c r="F65" s="164"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C65" s="163" t="s">
+        <v>325</v>
+      </c>
+      <c r="D65" s="198" t="s">
+        <v>311</v>
+      </c>
+      <c r="E65" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="F65" s="164" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B66" s="165"/>
+      <c r="C66" s="163" t="s">
+        <v>333</v>
+      </c>
+      <c r="D66" s="198" t="s">
+        <v>311</v>
+      </c>
+      <c r="E66" s="164" t="s">
+        <v>311</v>
+      </c>
+      <c r="F66" s="164" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B67" s="165"/>
@@ -8189,8 +8357,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{24287BB4-78F5-41D1-8279-0065565E5B4E}" topLeftCell="A46">
-      <selection activeCell="B16" sqref="B16"/>
+    <customSheetView guid="{BB5EAECB-8EEF-4DE2-9C73-C75A1E03B482}" showRuler="0" topLeftCell="A85">
+      <selection activeCell="A118" sqref="A118:G123"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
@@ -8201,14 +8369,30 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{BB5EAECB-8EEF-4DE2-9C73-C75A1E03B482}" showRuler="0" topLeftCell="A85">
-      <selection activeCell="A118" sqref="A118:G123"/>
+    <customSheetView guid="{24287BB4-78F5-41D1-8279-0065565E5B4E}" topLeftCell="A46">
+      <selection activeCell="B16" sqref="B16"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D26:D27"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C15:C16"/>
@@ -8219,22 +8403,6 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1">
@@ -8459,19 +8627,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Word.Document.8" shapeId="1025" r:id="rId7">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId8">
+          <objectPr defaultSize="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>4763</xdr:colOff>
                 <xdr:row>68</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3867150</xdr:colOff>
-                <xdr:row>86</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:colOff>3829050</xdr:colOff>
+                <xdr:row>120</xdr:row>
+                <xdr:rowOff>147638</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -8545,10 +8713,10 @@
       <c r="B5" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="231" t="s">
+      <c r="C5" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="230"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
@@ -8557,8 +8725,8 @@
       <c r="B6" s="42" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="231"/>
-      <c r="D6" s="230"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
@@ -8595,18 +8763,18 @@
       <c r="B10" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C10" s="231" t="s">
+      <c r="C10" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="230"/>
+      <c r="D10" s="229"/>
     </row>
     <row r="11" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="231"/>
-      <c r="D11" s="230"/>
+      <c r="C11" s="228"/>
+      <c r="D11" s="229"/>
     </row>
     <row r="12" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
@@ -8620,18 +8788,18 @@
       <c r="B13" s="216" t="s">
         <v>261</v>
       </c>
-      <c r="C13" s="231" t="s">
+      <c r="C13" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="230"/>
+      <c r="D13" s="229"/>
     </row>
     <row r="14" spans="1:6" s="215" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A14" s="145"/>
       <c r="B14" s="147" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="231"/>
-      <c r="D14" s="230"/>
+      <c r="C14" s="228"/>
+      <c r="D14" s="229"/>
     </row>
     <row r="15" spans="1:6" s="215" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="148"/>
@@ -8643,18 +8811,18 @@
       <c r="B16" s="149" t="s">
         <v>206</v>
       </c>
-      <c r="C16" s="231" t="s">
+      <c r="C16" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="230"/>
+      <c r="D16" s="229"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="150" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="231"/>
-      <c r="D17" s="230"/>
+      <c r="C17" s="228"/>
+      <c r="D17" s="229"/>
     </row>
     <row r="18" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
@@ -8685,26 +8853,26 @@
       <c r="B21" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="231" t="s">
+      <c r="C21" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="230"/>
+      <c r="D21" s="229"/>
     </row>
     <row r="22" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="231"/>
-      <c r="D22" s="230"/>
+      <c r="C22" s="228"/>
+      <c r="D22" s="229"/>
     </row>
     <row r="23" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="231"/>
-      <c r="D23" s="230"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="229"/>
     </row>
     <row r="24" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
@@ -8717,26 +8885,26 @@
       <c r="B25" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C25" s="231" t="s">
+      <c r="C25" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="230"/>
+      <c r="D25" s="229"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="231"/>
-      <c r="D26" s="230"/>
+      <c r="C26" s="228"/>
+      <c r="D26" s="229"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="231"/>
-      <c r="D27" s="230"/>
+      <c r="C27" s="228"/>
+      <c r="D27" s="229"/>
     </row>
     <row r="28" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
@@ -8765,18 +8933,18 @@
       <c r="B31" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="231" t="s">
+      <c r="C31" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="230"/>
+      <c r="D31" s="229"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="231"/>
-      <c r="D32" s="230"/>
+      <c r="C32" s="228"/>
+      <c r="D32" s="229"/>
     </row>
     <row r="33" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
@@ -8795,18 +8963,18 @@
       <c r="B35" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="231" t="s">
+      <c r="C35" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="230"/>
+      <c r="D35" s="229"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="231"/>
-      <c r="D36" s="230"/>
+      <c r="C36" s="228"/>
+      <c r="D36" s="229"/>
     </row>
     <row r="37" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
@@ -8819,18 +8987,18 @@
       <c r="B38" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C38" s="231" t="s">
+      <c r="C38" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="230"/>
+      <c r="D38" s="229"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="231"/>
-      <c r="D39" s="230"/>
+      <c r="C39" s="228"/>
+      <c r="D39" s="229"/>
     </row>
     <row r="40" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
@@ -8849,26 +9017,26 @@
       <c r="B42" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="231" t="s">
+      <c r="C42" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="230"/>
+      <c r="D42" s="229"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="231"/>
-      <c r="D43" s="230"/>
+      <c r="C43" s="228"/>
+      <c r="D43" s="229"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="231"/>
-      <c r="D44" s="230"/>
+      <c r="C44" s="228"/>
+      <c r="D44" s="229"/>
     </row>
     <row r="45" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
@@ -8917,18 +9085,18 @@
       <c r="B50" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="231" t="s">
+      <c r="C50" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="230"/>
+      <c r="D50" s="229"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="231"/>
-      <c r="D51" s="230"/>
+      <c r="C51" s="228"/>
+      <c r="D51" s="229"/>
     </row>
     <row r="52" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1"/>
@@ -8941,18 +9109,18 @@
       <c r="B53" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="231" t="s">
+      <c r="C53" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="230"/>
+      <c r="D53" s="229"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C54" s="231"/>
-      <c r="D54" s="230"/>
+      <c r="C54" s="228"/>
+      <c r="D54" s="229"/>
     </row>
     <row r="55" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="13"/>
@@ -8965,18 +9133,18 @@
       <c r="B56" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="231" t="s">
+      <c r="C56" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="230"/>
+      <c r="D56" s="229"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
       <c r="B57" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="230"/>
+      <c r="C57" s="228"/>
+      <c r="D57" s="229"/>
     </row>
     <row r="58" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13"/>
@@ -8989,18 +9157,18 @@
       <c r="B59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="231" t="s">
+      <c r="C59" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="230"/>
+      <c r="D59" s="229"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="13"/>
       <c r="B60" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="230"/>
+      <c r="C60" s="228"/>
+      <c r="D60" s="229"/>
     </row>
     <row r="61" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13"/>
@@ -9013,18 +9181,18 @@
       <c r="B62" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="231" t="s">
+      <c r="C62" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="230"/>
+      <c r="D62" s="229"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
       <c r="B63" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="231"/>
-      <c r="D63" s="230"/>
+      <c r="C63" s="228"/>
+      <c r="D63" s="229"/>
     </row>
     <row r="64" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
@@ -9037,18 +9205,18 @@
       <c r="B65" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C65" s="231" t="s">
+      <c r="C65" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="230"/>
+      <c r="D65" s="229"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="C66" s="231"/>
-      <c r="D66" s="230"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="229"/>
     </row>
     <row r="67" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
@@ -9061,18 +9229,18 @@
       <c r="B68" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="231" t="s">
+      <c r="C68" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D68" s="230"/>
+      <c r="D68" s="229"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="231"/>
-      <c r="D69" s="230"/>
+      <c r="C69" s="228"/>
+      <c r="D69" s="229"/>
     </row>
     <row r="70" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
@@ -9085,18 +9253,18 @@
       <c r="B71" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C71" s="231" t="s">
+      <c r="C71" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="230"/>
+      <c r="D71" s="229"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
       <c r="B72" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="231"/>
-      <c r="D72" s="230"/>
+      <c r="C72" s="228"/>
+      <c r="D72" s="229"/>
     </row>
     <row r="73" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
@@ -9109,18 +9277,18 @@
       <c r="B74" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C74" s="231" t="s">
+      <c r="C74" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D74" s="230"/>
+      <c r="D74" s="229"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="231"/>
-      <c r="D75" s="230"/>
+      <c r="C75" s="228"/>
+      <c r="D75" s="229"/>
     </row>
     <row r="76" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
@@ -9133,18 +9301,18 @@
       <c r="B77" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C77" s="231" t="s">
+      <c r="C77" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D77" s="230"/>
+      <c r="D77" s="229"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="13"/>
       <c r="B78" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="231"/>
-      <c r="D78" s="230"/>
+      <c r="C78" s="228"/>
+      <c r="D78" s="229"/>
     </row>
     <row r="79" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13"/>
@@ -9157,18 +9325,18 @@
       <c r="B80" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C80" s="231" t="s">
+      <c r="C80" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D80" s="230"/>
+      <c r="D80" s="229"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="13"/>
       <c r="B81" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C81" s="231"/>
-      <c r="D81" s="230"/>
+      <c r="C81" s="228"/>
+      <c r="D81" s="229"/>
     </row>
     <row r="82" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
@@ -9181,26 +9349,26 @@
       <c r="B83" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C83" s="231" t="s">
+      <c r="C83" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D83" s="230"/>
+      <c r="D83" s="229"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="13"/>
       <c r="B84" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C84" s="231"/>
-      <c r="D84" s="230"/>
+      <c r="C84" s="228"/>
+      <c r="D84" s="229"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="13"/>
       <c r="B85" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C85" s="231"/>
-      <c r="D85" s="230"/>
+      <c r="C85" s="228"/>
+      <c r="D85" s="229"/>
     </row>
     <row r="86" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
@@ -9213,26 +9381,26 @@
       <c r="B87" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="C87" s="231" t="s">
+      <c r="C87" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D87" s="230"/>
+      <c r="D87" s="229"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="13"/>
       <c r="B88" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C88" s="231"/>
-      <c r="D88" s="230"/>
+      <c r="C88" s="228"/>
+      <c r="D88" s="229"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
       <c r="B89" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C89" s="231"/>
-      <c r="D89" s="230"/>
+      <c r="C89" s="228"/>
+      <c r="D89" s="229"/>
     </row>
     <row r="90" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="13"/>
@@ -9243,7 +9411,7 @@
       <c r="B91" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="C91" s="232" t="s">
+      <c r="C91" s="230" t="s">
         <v>64</v>
       </c>
       <c r="D91" s="171"/>
@@ -9291,26 +9459,26 @@
       <c r="B97" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="231" t="s">
+      <c r="C97" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D97" s="230"/>
+      <c r="D97" s="229"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="B98" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="C98" s="231"/>
-      <c r="D98" s="230"/>
+      <c r="C98" s="228"/>
+      <c r="D98" s="229"/>
     </row>
     <row r="99" spans="1:4" ht="20.65" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
       <c r="B99" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="C99" s="231"/>
-      <c r="D99" s="230"/>
+      <c r="C99" s="228"/>
+      <c r="D99" s="229"/>
     </row>
     <row r="100" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="13"/>
@@ -9335,18 +9503,18 @@
       <c r="B102" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C102" s="231" t="s">
+      <c r="C102" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D102" s="230"/>
+      <c r="D102" s="229"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C103" s="231"/>
-      <c r="D103" s="230"/>
+      <c r="C103" s="228"/>
+      <c r="D103" s="229"/>
     </row>
     <row r="104" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1"/>
@@ -9371,18 +9539,18 @@
       <c r="B106" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C106" s="231" t="s">
+      <c r="C106" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D106" s="230"/>
+      <c r="D106" s="229"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="13"/>
       <c r="B107" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C107" s="231"/>
-      <c r="D107" s="230"/>
+      <c r="C107" s="228"/>
+      <c r="D107" s="229"/>
     </row>
     <row r="108" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1"/>
@@ -9395,18 +9563,18 @@
       <c r="B109" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C109" s="231" t="s">
+      <c r="C109" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D109" s="230"/>
+      <c r="D109" s="229"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="13"/>
       <c r="B110" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C110" s="231"/>
-      <c r="D110" s="230"/>
+      <c r="C110" s="228"/>
+      <c r="D110" s="229"/>
     </row>
     <row r="111" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1"/>
@@ -9419,26 +9587,26 @@
       <c r="B112" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C112" s="231" t="s">
+      <c r="C112" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D112" s="230"/>
+      <c r="D112" s="229"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="13"/>
       <c r="B113" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="C113" s="231"/>
-      <c r="D113" s="230"/>
+      <c r="C113" s="228"/>
+      <c r="D113" s="229"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="13"/>
       <c r="B114" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C114" s="231"/>
-      <c r="D114" s="230"/>
+      <c r="C114" s="228"/>
+      <c r="D114" s="229"/>
     </row>
     <row r="115" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="13"/>
@@ -9451,18 +9619,18 @@
       <c r="B116" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C116" s="231" t="s">
+      <c r="C116" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D116" s="230"/>
+      <c r="D116" s="229"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="13"/>
       <c r="B117" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C117" s="231"/>
-      <c r="D117" s="230"/>
+      <c r="C117" s="228"/>
+      <c r="D117" s="229"/>
     </row>
     <row r="118" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="13"/>
@@ -9475,18 +9643,18 @@
       <c r="B119" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C119" s="231" t="s">
+      <c r="C119" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D119" s="230"/>
+      <c r="D119" s="229"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="13"/>
       <c r="B120" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="C120" s="231"/>
-      <c r="D120" s="230"/>
+      <c r="C120" s="228"/>
+      <c r="D120" s="229"/>
     </row>
     <row r="121" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="13"/>
@@ -9499,18 +9667,18 @@
       <c r="B122" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C122" s="231" t="s">
+      <c r="C122" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D122" s="230"/>
+      <c r="D122" s="229"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="13"/>
       <c r="B123" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="231"/>
-      <c r="D123" s="230"/>
+      <c r="C123" s="228"/>
+      <c r="D123" s="229"/>
     </row>
     <row r="124" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="13"/>
@@ -9523,18 +9691,18 @@
       <c r="B125" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C125" s="231" t="s">
+      <c r="C125" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D125" s="230"/>
+      <c r="D125" s="229"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="13"/>
       <c r="B126" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C126" s="231"/>
-      <c r="D126" s="230"/>
+      <c r="C126" s="228"/>
+      <c r="D126" s="229"/>
     </row>
     <row r="127" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="13"/>
@@ -9559,18 +9727,18 @@
       <c r="B129" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="C129" s="231" t="s">
+      <c r="C129" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D129" s="230"/>
+      <c r="D129" s="229"/>
     </row>
     <row r="130" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="13"/>
       <c r="B130" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C130" s="231"/>
-      <c r="D130" s="230"/>
+      <c r="C130" s="228"/>
+      <c r="D130" s="229"/>
     </row>
     <row r="131" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="13"/>
@@ -9583,18 +9751,18 @@
       <c r="B132" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C132" s="231" t="s">
+      <c r="C132" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D132" s="230"/>
+      <c r="D132" s="229"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="13"/>
       <c r="B133" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C133" s="231"/>
-      <c r="D133" s="230"/>
+      <c r="C133" s="228"/>
+      <c r="D133" s="229"/>
     </row>
     <row r="134" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="13"/>
@@ -9607,18 +9775,18 @@
       <c r="B135" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="C135" s="231" t="s">
+      <c r="C135" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D135" s="230"/>
+      <c r="D135" s="229"/>
     </row>
     <row r="136" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="13"/>
       <c r="B136" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C136" s="231"/>
-      <c r="D136" s="230"/>
+      <c r="C136" s="228"/>
+      <c r="D136" s="229"/>
     </row>
     <row r="137" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="13"/>
@@ -9631,18 +9799,18 @@
       <c r="B138" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C138" s="231" t="s">
+      <c r="C138" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D138" s="230"/>
+      <c r="D138" s="229"/>
     </row>
     <row r="139" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="13"/>
       <c r="B139" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C139" s="231"/>
-      <c r="D139" s="230"/>
+      <c r="C139" s="228"/>
+      <c r="D139" s="229"/>
     </row>
     <row r="140" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
@@ -9655,18 +9823,18 @@
       <c r="B141" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C141" s="231" t="s">
+      <c r="C141" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D141" s="230"/>
+      <c r="D141" s="229"/>
     </row>
     <row r="142" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="13"/>
       <c r="B142" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C142" s="231"/>
-      <c r="D142" s="230"/>
+      <c r="C142" s="228"/>
+      <c r="D142" s="229"/>
     </row>
     <row r="143" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
@@ -9679,18 +9847,18 @@
       <c r="B144" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C144" s="231" t="s">
+      <c r="C144" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D144" s="230"/>
+      <c r="D144" s="229"/>
     </row>
     <row r="145" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="13"/>
       <c r="B145" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C145" s="231"/>
-      <c r="D145" s="230"/>
+      <c r="C145" s="228"/>
+      <c r="D145" s="229"/>
     </row>
     <row r="146" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
@@ -9715,18 +9883,18 @@
       <c r="B148" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C148" s="231" t="s">
+      <c r="C148" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D148" s="230"/>
+      <c r="D148" s="229"/>
     </row>
     <row r="149" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="13"/>
       <c r="B149" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C149" s="231"/>
-      <c r="D149" s="230"/>
+      <c r="C149" s="228"/>
+      <c r="D149" s="229"/>
     </row>
     <row r="150" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="13"/>
@@ -9751,18 +9919,18 @@
       <c r="B152" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C152" s="231" t="s">
+      <c r="C152" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D152" s="230"/>
+      <c r="D152" s="229"/>
     </row>
     <row r="153" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="13"/>
       <c r="B153" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C153" s="231"/>
-      <c r="D153" s="230"/>
+      <c r="C153" s="228"/>
+      <c r="D153" s="229"/>
     </row>
     <row r="154" spans="1:4" s="45" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B154" s="47"/>
@@ -9978,6 +10146,75 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="81">
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="D87:D89"/>
+    <mergeCell ref="C91:C95"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="D132:D133"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="D135:D136"/>
     <mergeCell ref="C138:C139"/>
@@ -9990,75 +10227,6 @@
     <mergeCell ref="D144:D145"/>
     <mergeCell ref="C148:C149"/>
     <mergeCell ref="D148:D149"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="C129:C130"/>
-    <mergeCell ref="D129:D130"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="D119:D120"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="C91:C95"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="D102:D103"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="C87:C89"/>
-    <mergeCell ref="D87:D89"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1">
@@ -10850,10 +11018,10 @@
       <c r="B17" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="231" t="s">
+      <c r="C17" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="230"/>
+      <c r="D17" s="229"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -10864,8 +11032,8 @@
       <c r="B18" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="231"/>
-      <c r="D18" s="230"/>
+      <c r="C18" s="228"/>
+      <c r="D18" s="229"/>
     </row>
     <row r="19" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
@@ -10877,18 +11045,18 @@
       <c r="B20" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C20" s="231" t="s">
+      <c r="C20" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="230"/>
+      <c r="D20" s="229"/>
     </row>
     <row r="21" spans="1:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="C21" s="231"/>
-      <c r="D21" s="230"/>
+      <c r="C21" s="228"/>
+      <c r="D21" s="229"/>
     </row>
     <row r="22" spans="1:8" ht="6.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
@@ -10902,18 +11070,18 @@
       <c r="B23" s="216" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="231" t="s">
+      <c r="C23" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="230"/>
+      <c r="D23" s="229"/>
     </row>
     <row r="24" spans="1:8" s="215" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A24" s="145"/>
       <c r="B24" s="147" t="s">
         <v>262</v>
       </c>
-      <c r="C24" s="231"/>
-      <c r="D24" s="230"/>
+      <c r="C24" s="228"/>
+      <c r="D24" s="229"/>
     </row>
     <row r="25" spans="1:8" s="215" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="148"/>
@@ -10924,10 +11092,10 @@
       <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="231" t="s">
+      <c r="C26" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="230"/>
+      <c r="D26" s="229"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -10938,8 +11106,8 @@
       <c r="B27" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="C27" s="231"/>
-      <c r="D27" s="230"/>
+      <c r="C27" s="228"/>
+      <c r="D27" s="229"/>
     </row>
     <row r="28" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
@@ -10950,10 +11118,10 @@
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="231" t="s">
+      <c r="C29" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="230"/>
+      <c r="D29" s="229"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -10964,8 +11132,8 @@
       <c r="B30" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="C30" s="231"/>
-      <c r="D30" s="230"/>
+      <c r="C30" s="228"/>
+      <c r="D30" s="229"/>
     </row>
     <row r="31" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
@@ -10980,10 +11148,10 @@
       <c r="B32" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C32" s="231" t="s">
+      <c r="C32" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="230"/>
+      <c r="D32" s="229"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -10994,8 +11162,8 @@
       <c r="B33" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="231"/>
-      <c r="D33" s="230"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="229"/>
     </row>
     <row r="34" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
@@ -11011,10 +11179,10 @@
       <c r="B35" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C35" s="231" t="s">
+      <c r="C35" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="230"/>
+      <c r="D35" s="229"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -11025,8 +11193,8 @@
       <c r="B36" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C36" s="231"/>
-      <c r="D36" s="230"/>
+      <c r="C36" s="228"/>
+      <c r="D36" s="229"/>
     </row>
     <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
@@ -11038,10 +11206,10 @@
       <c r="B38" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="231" t="s">
+      <c r="C38" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="230"/>
+      <c r="D38" s="229"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
@@ -11052,8 +11220,8 @@
       <c r="B39" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="C39" s="231"/>
-      <c r="D39" s="230"/>
+      <c r="C39" s="228"/>
+      <c r="D39" s="229"/>
     </row>
     <row r="40" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
@@ -11082,18 +11250,18 @@
       <c r="B42" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="231" t="s">
+      <c r="C42" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="230"/>
+      <c r="D42" s="229"/>
     </row>
     <row r="43" spans="1:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A43" s="3"/>
       <c r="B43" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="231"/>
-      <c r="D43" s="230"/>
+      <c r="C43" s="228"/>
+      <c r="D43" s="229"/>
     </row>
     <row r="44" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3"/>
@@ -11105,25 +11273,25 @@
       <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="231" t="s">
+      <c r="C45" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="233"/>
+      <c r="D45" s="231"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C46" s="231"/>
-      <c r="D46" s="234"/>
+      <c r="C46" s="228"/>
+      <c r="D46" s="232"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C47" s="231"/>
+      <c r="C47" s="228"/>
       <c r="D47" s="171"/>
     </row>
     <row r="48" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
@@ -11136,18 +11304,18 @@
       <c r="B49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="231" t="s">
+      <c r="C49" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D49" s="230"/>
+      <c r="D49" s="229"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="231"/>
-      <c r="D50" s="230"/>
+      <c r="C50" s="228"/>
+      <c r="D50" s="229"/>
     </row>
     <row r="51" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
@@ -11160,18 +11328,18 @@
       <c r="B52" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C52" s="231" t="s">
+      <c r="C52" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="230"/>
+      <c r="D52" s="229"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="13"/>
       <c r="B53" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="C53" s="231"/>
-      <c r="D53" s="230"/>
+      <c r="C53" s="228"/>
+      <c r="D53" s="229"/>
     </row>
     <row r="54" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
@@ -11194,18 +11362,18 @@
       <c r="B56" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="C56" s="231" t="s">
+      <c r="C56" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="230"/>
+      <c r="D56" s="229"/>
     </row>
     <row r="57" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A57" s="3"/>
       <c r="B57" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C57" s="231"/>
-      <c r="D57" s="230"/>
+      <c r="C57" s="228"/>
+      <c r="D57" s="229"/>
     </row>
     <row r="58" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3"/>
@@ -11217,18 +11385,18 @@
       <c r="B59" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="231" t="s">
+      <c r="C59" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="230"/>
+      <c r="D59" s="229"/>
     </row>
     <row r="60" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A60" s="3"/>
       <c r="B60" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="230"/>
+      <c r="C60" s="228"/>
+      <c r="D60" s="229"/>
     </row>
     <row r="61" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3"/>
@@ -11240,18 +11408,18 @@
       <c r="B62" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="231" t="s">
+      <c r="C62" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="230"/>
+      <c r="D62" s="229"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
       <c r="B63" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="231"/>
-      <c r="D63" s="230"/>
+      <c r="C63" s="228"/>
+      <c r="D63" s="229"/>
     </row>
     <row r="64" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
@@ -11263,25 +11431,25 @@
       <c r="B65" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C65" s="231" t="s">
+      <c r="C65" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="233"/>
+      <c r="D65" s="231"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="C66" s="231"/>
-      <c r="D66" s="234"/>
+      <c r="C66" s="228"/>
+      <c r="D66" s="232"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="C67" s="231"/>
+      <c r="C67" s="228"/>
       <c r="D67" s="171"/>
     </row>
     <row r="68" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
@@ -11306,18 +11474,18 @@
       <c r="B70" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="C70" s="231" t="s">
+      <c r="C70" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D70" s="230"/>
+      <c r="D70" s="229"/>
     </row>
     <row r="71" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A71" s="3"/>
       <c r="B71" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C71" s="231"/>
-      <c r="D71" s="230"/>
+      <c r="C71" s="228"/>
+      <c r="D71" s="229"/>
     </row>
     <row r="72" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3"/>
@@ -11329,18 +11497,18 @@
       <c r="B73" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="231" t="s">
+      <c r="C73" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D73" s="230"/>
+      <c r="D73" s="229"/>
     </row>
     <row r="74" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A74" s="3"/>
       <c r="B74" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C74" s="231"/>
-      <c r="D74" s="230"/>
+      <c r="C74" s="228"/>
+      <c r="D74" s="229"/>
     </row>
     <row r="75" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3"/>
@@ -11395,18 +11563,18 @@
       <c r="B81" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="C81" s="231" t="s">
+      <c r="C81" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="230"/>
+      <c r="D81" s="229"/>
     </row>
     <row r="82" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A82" s="3"/>
       <c r="B82" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C82" s="231"/>
-      <c r="D82" s="230"/>
+      <c r="C82" s="228"/>
+      <c r="D82" s="229"/>
     </row>
     <row r="83" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3"/>
@@ -11418,18 +11586,18 @@
       <c r="B84" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C84" s="231" t="s">
+      <c r="C84" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D84" s="230"/>
+      <c r="D84" s="229"/>
     </row>
     <row r="85" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A85" s="3"/>
       <c r="B85" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="C85" s="231"/>
-      <c r="D85" s="230"/>
+      <c r="C85" s="228"/>
+      <c r="D85" s="229"/>
     </row>
     <row r="86" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3"/>
@@ -11440,10 +11608,10 @@
       <c r="B87" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C87" s="231" t="s">
+      <c r="C87" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D87" s="230"/>
+      <c r="D87" s="229"/>
       <c r="E87" s="32"/>
       <c r="F87" s="32"/>
     </row>
@@ -11452,8 +11620,8 @@
       <c r="B88" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C88" s="231"/>
-      <c r="D88" s="230"/>
+      <c r="C88" s="228"/>
+      <c r="D88" s="229"/>
     </row>
     <row r="89" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3"/>
@@ -11480,18 +11648,18 @@
       <c r="B91" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C91" s="231" t="s">
+      <c r="C91" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D91" s="230"/>
+      <c r="D91" s="229"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="13"/>
       <c r="B92" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="231"/>
-      <c r="D92" s="230"/>
+      <c r="C92" s="228"/>
+      <c r="D92" s="229"/>
     </row>
     <row r="93" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3"/>
@@ -11503,18 +11671,18 @@
       <c r="B94" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C94" s="231" t="s">
+      <c r="C94" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D94" s="230"/>
+      <c r="D94" s="229"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="13"/>
       <c r="B95" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C95" s="231"/>
-      <c r="D95" s="230"/>
+      <c r="C95" s="228"/>
+      <c r="D95" s="229"/>
     </row>
     <row r="96" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3"/>
@@ -11526,18 +11694,18 @@
       <c r="B97" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C97" s="231" t="s">
+      <c r="C97" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D97" s="230"/>
+      <c r="D97" s="229"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="B98" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C98" s="231"/>
-      <c r="D98" s="230"/>
+      <c r="C98" s="228"/>
+      <c r="D98" s="229"/>
     </row>
     <row r="99" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
@@ -11561,18 +11729,18 @@
       <c r="B101" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C101" s="231" t="s">
+      <c r="C101" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D101" s="230"/>
+      <c r="D101" s="229"/>
     </row>
     <row r="102" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3"/>
       <c r="B102" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C102" s="231"/>
-      <c r="D102" s="230"/>
+      <c r="C102" s="228"/>
+      <c r="D102" s="229"/>
     </row>
     <row r="103" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3"/>
@@ -11599,18 +11767,18 @@
       <c r="B106" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C106" s="231" t="s">
+      <c r="C106" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D106" s="230"/>
+      <c r="D106" s="229"/>
     </row>
     <row r="107" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A107" s="3"/>
       <c r="B107" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C107" s="231"/>
-      <c r="D107" s="230"/>
+      <c r="C107" s="228"/>
+      <c r="D107" s="229"/>
     </row>
     <row r="108" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3"/>
@@ -11622,18 +11790,18 @@
       <c r="B109" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C109" s="231" t="s">
+      <c r="C109" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D109" s="230"/>
+      <c r="D109" s="229"/>
     </row>
     <row r="110" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A110" s="3"/>
       <c r="B110" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C110" s="231"/>
-      <c r="D110" s="230"/>
+      <c r="C110" s="228"/>
+      <c r="D110" s="229"/>
     </row>
     <row r="111" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="13"/>
@@ -11658,18 +11826,18 @@
       <c r="B113" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C113" s="231" t="s">
+      <c r="C113" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D113" s="230"/>
+      <c r="D113" s="229"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="13"/>
       <c r="B114" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C114" s="231"/>
-      <c r="D114" s="230"/>
+      <c r="C114" s="228"/>
+      <c r="D114" s="229"/>
     </row>
     <row r="115" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="13"/>
@@ -11706,18 +11874,18 @@
       <c r="B118" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C118" s="231" t="s">
+      <c r="C118" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D118" s="230"/>
+      <c r="D118" s="229"/>
     </row>
     <row r="119" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="13"/>
       <c r="B119" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C119" s="231"/>
-      <c r="D119" s="230"/>
+      <c r="C119" s="228"/>
+      <c r="D119" s="229"/>
     </row>
     <row r="120" spans="1:6" s="45" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="47"/>
@@ -11912,24 +12080,32 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="58">
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:D66"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C26:C27"/>
@@ -11944,32 +12120,24 @@
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C45:C47"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A1:B1 D1">
@@ -12565,18 +12733,18 @@
       <c r="B8" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="231" t="s">
+      <c r="C8" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="230"/>
+      <c r="D8" s="229"/>
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="231"/>
-      <c r="D9" s="230"/>
+      <c r="C9" s="228"/>
+      <c r="D9" s="229"/>
     </row>
     <row r="10" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
@@ -12701,18 +12869,18 @@
       <c r="B25" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="231" t="s">
+      <c r="C25" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="230"/>
+      <c r="D25" s="229"/>
     </row>
     <row r="26" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="231"/>
-      <c r="D26" s="230"/>
+      <c r="C26" s="228"/>
+      <c r="D26" s="229"/>
     </row>
     <row r="27" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
@@ -12741,10 +12909,10 @@
       <c r="B30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="235" t="s">
+      <c r="C30" s="233" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="236"/>
+      <c r="D30" s="234"/>
     </row>
     <row r="31" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
@@ -12768,18 +12936,18 @@
       <c r="B33" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="231" t="s">
+      <c r="C33" s="228" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="230"/>
+      <c r="D33" s="229"/>
     </row>
     <row r="34" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="231"/>
-      <c r="D34" s="230"/>
+      <c r="C34" s="228"/>
+      <c r="D34" s="229"/>
     </row>
     <row r="35" spans="1:6" s="45" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
@@ -13204,6 +13372,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3268A085264BF48BD37900163DF0D2E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29a7b4972ef9a00e6ec0766ab6c4dc18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -13252,32 +13435,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05CF8F61-890E-4D58-B63E-404A8F71F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4C9B69C-ACD7-403C-A39C-3C738D5910B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13297,9 +13458,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4C9B69C-ACD7-403C-A39C-3C738D5910B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05CF8F61-890E-4D58-B63E-404A8F71F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>